<commit_message>
separacion de almacenes liquidos y jarcieria
separacion de almacenes liquidos y jarcieria en app, tambien se separa el consulta compras desde sp ya que se compartia con el admin
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Observaciones Jessy 26052021.xlsx
+++ b/Analisis/SPRINTs/Observaciones Jessy 26052021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91784AE7-8A86-408E-802A-62017C424217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3E4A98-8A15-4E56-A841-C516DF59DD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="765" windowWidth="22935" windowHeight="11580" xr2:uid="{C2C6F7BE-A971-480C-B953-016E6C6E6AD6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C2C6F7BE-A971-480C-B953-016E6C6E6AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>TiendasAlmacen</t>
   </si>
@@ -114,9 +114,6 @@
     <t>[SP_APP_OBTENER_NOTIFICACIONES_PEDIDOS_INTERNOS]</t>
   </si>
   <si>
-    <t>SP_APP_OBTENER_NOTIFICACIONES_PEDIDOS_INTERNOS</t>
-  </si>
-  <si>
     <t>@idTipoPedidoInterno</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>Crear Tablas del excel</t>
+  </si>
+  <si>
+    <t>no es necesario ya que desde que se genera el pedido sabes que almacen esta solicitando por lo tanto no podria ver de otros almacenes</t>
   </si>
 </sst>
 </file>
@@ -228,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +238,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,13 +266,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE72AFA4-1FE2-4591-B110-617832DD8F2C}">
-  <dimension ref="B1:N57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B43" sqref="B43:J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,13 +601,13 @@
     <col min="9" max="9" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="J1" t="s">
         <v>5</v>
       </c>
@@ -601,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -633,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>4</v>
       </c>
@@ -643,9 +657,9 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44343</v>
+        <v>44348</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -666,7 +680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>4</v>
       </c>
@@ -676,9 +690,9 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f ca="1">TODAY()</f>
-        <v>44343</v>
+        <v>44348</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -699,7 +713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>6</v>
       </c>
@@ -709,9 +723,9 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f ca="1">TODAY()</f>
-        <v>44343</v>
+        <v>44348</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -729,21 +743,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H6" s="2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
         <v>4</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>3</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H7">
         <v>5</v>
       </c>
@@ -754,18 +768,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H8" s="2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
         <v>6</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -773,246 +787,222 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>45</v>
       </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>20</v>
       </c>
       <c r="I14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
         <v>48</v>
       </c>
-      <c r="J14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="I15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="I17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
         <v>53</v>
       </c>
-      <c r="J17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I18" t="s">
+      <c r="J18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
         <v>54</v>
       </c>
-      <c r="J18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I19" t="s">
-        <v>55</v>
-      </c>
       <c r="J19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>27</v>
       </c>
       <c r="I21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="I22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>25</v>
       </c>
       <c r="I23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
@@ -1022,17 +1012,17 @@
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>